<commit_message>
kleine wijzigingen blanco excel
</commit_message>
<xml_diff>
--- a/_data/ni/individueel_eindstand_blanco_v5.xlsx
+++ b/_data/ni/individueel_eindstand_blanco_v5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="6420" windowWidth="14340" windowHeight="6435"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="14355" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="16" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="47">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -165,6 +165,9 @@
   <si>
     <t>matchpunten: w 3 - g 2 - v 1 - vf 0</t>
   </si>
+  <si>
+    <t>blanco versie 5</t>
+  </si>
 </sst>
 </file>
 
@@ -174,7 +177,7 @@
     <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +259,15 @@
       <b/>
       <sz val="11"/>
       <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -785,7 +797,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1009,6 +1021,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1312,7 +1325,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1326,7 +1341,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+      <c r="A2" s="85" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="3" spans="1:2">
       <c r="A3" s="71" t="s">
         <v>0</v>
@@ -3237,7 +3256,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="24" customWidth="1"/>
     <col min="3" max="14" width="4" style="24" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5.42578125" style="24" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="5.42578125" style="24" customWidth="1"/>
@@ -3278,51 +3297,51 @@
         <v>33</v>
       </c>
       <c r="C3" s="28">
-        <f>MATCH("XX",C4:C15,0)</f>
+        <f t="shared" ref="C3:N3" si="0">MATCH("XX",C4:C15,0)</f>
         <v>1</v>
       </c>
       <c r="D3" s="28">
-        <f>MATCH("XX",D4:D15,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E3" s="28">
-        <f>MATCH("XX",E4:E15,0)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F3" s="28">
-        <f>MATCH("XX",F4:F15,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G3" s="28">
-        <f>MATCH("XX",G4:G15,0)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="H3" s="28">
-        <f>MATCH("XX",H4:H15,0)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I3" s="28">
-        <f>MATCH("XX",I4:I15,0)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="J3" s="28">
-        <f>MATCH("XX",J4:J15,0)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="K3" s="28">
-        <f>MATCH("XX",K4:K15,0)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="L3" s="28">
-        <f>MATCH("XX",L4:L15,0)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="M3" s="28">
-        <f>MATCH("XX",M4:M15,0)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="N3" s="28">
-        <f>MATCH("XX",N4:N15,0)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="O3" s="29" t="s">
@@ -3367,7 +3386,7 @@
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
       <c r="O4" s="35">
-        <f>SUM(C4:N4)</f>
+        <f t="shared" ref="O4:O15" si="1">SUM(C4:N4)</f>
         <v>0</v>
       </c>
       <c r="P4" s="36">
@@ -3375,7 +3394,7 @@
         <v>0</v>
       </c>
       <c r="Q4" s="36">
-        <f>COUNT(C4:N4)</f>
+        <f t="shared" ref="Q4:Q15" si="2">COUNT(C4:N4)</f>
         <v>0</v>
       </c>
       <c r="R4" s="45"/>
@@ -3477,47 +3496,47 @@
         <v>37</v>
       </c>
       <c r="AT4" s="75" t="str">
-        <f>IF(T4="","",IF(D4=0,0,1+2*T4))</f>
+        <f t="shared" ref="AT4:BD4" si="3">IF(T4="","",IF(D4=0,0,1+2*T4))</f>
         <v/>
       </c>
       <c r="AU4" s="75" t="str">
-        <f>IF(U4="","",IF(E4=0,0,1+2*U4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AV4" s="75" t="str">
-        <f>IF(V4="","",IF(F4=0,0,1+2*V4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AW4" s="75" t="str">
-        <f>IF(W4="","",IF(G4=0,0,1+2*W4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AX4" s="75" t="str">
-        <f>IF(X4="","",IF(H4=0,0,1+2*X4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AY4" s="75" t="str">
-        <f>IF(Y4="","",IF(I4=0,0,1+2*Y4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="AZ4" s="75" t="str">
-        <f>IF(Z4="","",IF(J4=0,0,1+2*Z4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="BA4" s="75" t="str">
-        <f>IF(AA4="","",IF(K4=0,0,1+2*AA4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="BB4" s="75" t="str">
-        <f>IF(AB4="","",IF(L4=0,0,1+2*AB4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="BC4" s="75" t="str">
-        <f>IF(AC4="","",IF(M4=0,0,1+2*AC4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="BD4" s="76" t="str">
-        <f>IF(AD4="","",IF(N4=0,0,1+2*AD4))</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -3541,7 +3560,7 @@
       <c r="M5" s="34"/>
       <c r="N5" s="34"/>
       <c r="O5" s="35">
-        <f>SUM(C5:N5)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P5" s="36">
@@ -3549,7 +3568,7 @@
         <v>0</v>
       </c>
       <c r="Q5" s="36">
-        <f>COUNT(C5:N5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R5" s="45"/>
@@ -3648,50 +3667,50 @@
         <v>0</v>
       </c>
       <c r="AS5" s="77" t="str">
-        <f>IF(S5="","",IF(C5=0,0,1+2*S5))</f>
+        <f t="shared" ref="AS5:AS15" si="4">IF(S5="","",IF(C5=0,0,1+2*S5))</f>
         <v/>
       </c>
       <c r="AT5" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AU5" s="78" t="str">
-        <f>IF(U5="","",IF(E5=0,0,1+2*U5))</f>
+        <f t="shared" ref="AU5:BD5" si="5">IF(U5="","",IF(E5=0,0,1+2*U5))</f>
         <v/>
       </c>
       <c r="AV5" s="78" t="str">
-        <f>IF(V5="","",IF(F5=0,0,1+2*V5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AW5" s="78" t="str">
-        <f>IF(W5="","",IF(G5=0,0,1+2*W5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AX5" s="78" t="str">
-        <f>IF(X5="","",IF(H5=0,0,1+2*X5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AY5" s="78" t="str">
-        <f>IF(Y5="","",IF(I5=0,0,1+2*Y5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AZ5" s="78" t="str">
-        <f>IF(Z5="","",IF(J5=0,0,1+2*Z5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="BA5" s="78" t="str">
-        <f>IF(AA5="","",IF(K5=0,0,1+2*AA5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="BB5" s="78" t="str">
-        <f>IF(AB5="","",IF(L5=0,0,1+2*AB5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="BC5" s="78" t="str">
-        <f>IF(AC5="","",IF(M5=0,0,1+2*AC5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="BD5" s="79" t="str">
-        <f>IF(AD5="","",IF(N5=0,0,1+2*AD5))</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -3715,7 +3734,7 @@
       <c r="M6" s="34"/>
       <c r="N6" s="34"/>
       <c r="O6" s="35">
-        <f>SUM(C6:N6)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P6" s="36">
@@ -3723,7 +3742,7 @@
         <v>0</v>
       </c>
       <c r="Q6" s="36">
-        <f>COUNT(C6:N6)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R6" s="45"/>
@@ -3822,50 +3841,50 @@
         <v>0</v>
       </c>
       <c r="AS6" s="77" t="str">
-        <f>IF(S6="","",IF(C6=0,0,1+2*S6))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT6" s="78" t="str">
-        <f>IF(T6="","",IF(D6=0,0,1+2*T6))</f>
+        <f t="shared" ref="AT6:AT15" si="6">IF(T6="","",IF(D6=0,0,1+2*T6))</f>
         <v/>
       </c>
       <c r="AU6" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AV6" s="78" t="str">
-        <f>IF(V6="","",IF(F6=0,0,1+2*V6))</f>
+        <f t="shared" ref="AV6:BD6" si="7">IF(V6="","",IF(F6=0,0,1+2*V6))</f>
         <v/>
       </c>
       <c r="AW6" s="78" t="str">
-        <f>IF(W6="","",IF(G6=0,0,1+2*W6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AX6" s="78" t="str">
-        <f>IF(X6="","",IF(H6=0,0,1+2*X6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AY6" s="78" t="str">
-        <f>IF(Y6="","",IF(I6=0,0,1+2*Y6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AZ6" s="78" t="str">
-        <f>IF(Z6="","",IF(J6=0,0,1+2*Z6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="BA6" s="78" t="str">
-        <f>IF(AA6="","",IF(K6=0,0,1+2*AA6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="BB6" s="78" t="str">
-        <f>IF(AB6="","",IF(L6=0,0,1+2*AB6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="BC6" s="78" t="str">
-        <f>IF(AC6="","",IF(M6=0,0,1+2*AC6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="BD6" s="79" t="str">
-        <f>IF(AD6="","",IF(N6=0,0,1+2*AD6))</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -3889,7 +3908,7 @@
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
       <c r="O7" s="35">
-        <f>SUM(C7:N7)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P7" s="36">
@@ -3897,7 +3916,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="36">
-        <f>COUNT(C7:N7)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R7" s="45"/>
@@ -3996,50 +4015,50 @@
         <v>0</v>
       </c>
       <c r="AS7" s="77" t="str">
-        <f>IF(S7="","",IF(C7=0,0,1+2*S7))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT7" s="78" t="str">
-        <f>IF(T7="","",IF(D7=0,0,1+2*T7))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU7" s="78" t="str">
-        <f>IF(U7="","",IF(E7=0,0,1+2*U7))</f>
+        <f t="shared" ref="AU7:AU15" si="8">IF(U7="","",IF(E7=0,0,1+2*U7))</f>
         <v/>
       </c>
       <c r="AV7" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AW7" s="78" t="str">
-        <f>IF(W7="","",IF(G7=0,0,1+2*W7))</f>
+        <f t="shared" ref="AW7:BD7" si="9">IF(W7="","",IF(G7=0,0,1+2*W7))</f>
         <v/>
       </c>
       <c r="AX7" s="78" t="str">
-        <f>IF(X7="","",IF(H7=0,0,1+2*X7))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AY7" s="78" t="str">
-        <f>IF(Y7="","",IF(I7=0,0,1+2*Y7))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AZ7" s="78" t="str">
-        <f>IF(Z7="","",IF(J7=0,0,1+2*Z7))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="BA7" s="78" t="str">
-        <f>IF(AA7="","",IF(K7=0,0,1+2*AA7))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="BB7" s="78" t="str">
-        <f>IF(AB7="","",IF(L7=0,0,1+2*AB7))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="BC7" s="78" t="str">
-        <f>IF(AC7="","",IF(M7=0,0,1+2*AC7))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="BD7" s="79" t="str">
-        <f>IF(AD7="","",IF(N7=0,0,1+2*AD7))</f>
+        <f t="shared" si="9"/>
         <v/>
       </c>
     </row>
@@ -4063,7 +4082,7 @@
       <c r="M8" s="34"/>
       <c r="N8" s="34"/>
       <c r="O8" s="35">
-        <f>SUM(C8:N8)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P8" s="36">
@@ -4071,7 +4090,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="36">
-        <f>COUNT(C8:N8)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R8" s="45"/>
@@ -4170,50 +4189,50 @@
         <v>0</v>
       </c>
       <c r="AS8" s="77" t="str">
-        <f>IF(S8="","",IF(C8=0,0,1+2*S8))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT8" s="78" t="str">
-        <f>IF(T8="","",IF(D8=0,0,1+2*T8))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU8" s="78" t="str">
-        <f>IF(U8="","",IF(E8=0,0,1+2*U8))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV8" s="78" t="str">
-        <f>IF(V8="","",IF(F8=0,0,1+2*V8))</f>
+        <f t="shared" ref="AV8:AV15" si="10">IF(V8="","",IF(F8=0,0,1+2*V8))</f>
         <v/>
       </c>
       <c r="AW8" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AX8" s="78" t="str">
-        <f>IF(X8="","",IF(H8=0,0,1+2*X8))</f>
+        <f t="shared" ref="AX8:BD8" si="11">IF(X8="","",IF(H8=0,0,1+2*X8))</f>
         <v/>
       </c>
       <c r="AY8" s="78" t="str">
-        <f>IF(Y8="","",IF(I8=0,0,1+2*Y8))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="AZ8" s="78" t="str">
-        <f>IF(Z8="","",IF(J8=0,0,1+2*Z8))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BA8" s="78" t="str">
-        <f>IF(AA8="","",IF(K8=0,0,1+2*AA8))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BB8" s="78" t="str">
-        <f>IF(AB8="","",IF(L8=0,0,1+2*AB8))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BC8" s="78" t="str">
-        <f>IF(AC8="","",IF(M8=0,0,1+2*AC8))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="BD8" s="79" t="str">
-        <f>IF(AD8="","",IF(N8=0,0,1+2*AD8))</f>
+        <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
@@ -4237,7 +4256,7 @@
       <c r="M9" s="34"/>
       <c r="N9" s="34"/>
       <c r="O9" s="35">
-        <f>SUM(C9:N9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P9" s="36">
@@ -4245,7 +4264,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="36">
-        <f>COUNT(C9:N9)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R9" s="45"/>
@@ -4344,50 +4363,50 @@
         <v>0</v>
       </c>
       <c r="AS9" s="77" t="str">
-        <f>IF(S9="","",IF(C9=0,0,1+2*S9))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT9" s="78" t="str">
-        <f>IF(T9="","",IF(D9=0,0,1+2*T9))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU9" s="78" t="str">
-        <f>IF(U9="","",IF(E9=0,0,1+2*U9))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV9" s="78" t="str">
-        <f>IF(V9="","",IF(F9=0,0,1+2*V9))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AW9" s="78" t="str">
-        <f>IF(W9="","",IF(G9=0,0,1+2*W9))</f>
+        <f t="shared" ref="AW9:AW15" si="12">IF(W9="","",IF(G9=0,0,1+2*W9))</f>
         <v/>
       </c>
       <c r="AX9" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AY9" s="78" t="str">
-        <f>IF(Y9="","",IF(I9=0,0,1+2*Y9))</f>
+        <f t="shared" ref="AY9:BD9" si="13">IF(Y9="","",IF(I9=0,0,1+2*Y9))</f>
         <v/>
       </c>
       <c r="AZ9" s="78" t="str">
-        <f>IF(Z9="","",IF(J9=0,0,1+2*Z9))</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BA9" s="78" t="str">
-        <f>IF(AA9="","",IF(K9=0,0,1+2*AA9))</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BB9" s="78" t="str">
-        <f>IF(AB9="","",IF(L9=0,0,1+2*AB9))</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BC9" s="78" t="str">
-        <f>IF(AC9="","",IF(M9=0,0,1+2*AC9))</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="BD9" s="79" t="str">
-        <f>IF(AD9="","",IF(N9=0,0,1+2*AD9))</f>
+        <f t="shared" si="13"/>
         <v/>
       </c>
     </row>
@@ -4411,7 +4430,7 @@
       <c r="M10" s="34"/>
       <c r="N10" s="34"/>
       <c r="O10" s="35">
-        <f>SUM(C10:N10)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P10" s="36">
@@ -4419,7 +4438,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="36">
-        <f>COUNT(C10:N10)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R10" s="45"/>
@@ -4518,27 +4537,27 @@
         <v>0</v>
       </c>
       <c r="AS10" s="77" t="str">
-        <f>IF(S10="","",IF(C10=0,0,1+2*S10))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT10" s="78" t="str">
-        <f>IF(T10="","",IF(D10=0,0,1+2*T10))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU10" s="78" t="str">
-        <f>IF(U10="","",IF(E10=0,0,1+2*U10))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV10" s="78" t="str">
-        <f>IF(V10="","",IF(F10=0,0,1+2*V10))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AW10" s="78" t="str">
-        <f>IF(W10="","",IF(G10=0,0,1+2*W10))</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AX10" s="78" t="str">
-        <f>IF(X10="","",IF(H10=0,0,1+2*X10))</f>
+        <f t="shared" ref="AX10:AX15" si="14">IF(X10="","",IF(H10=0,0,1+2*X10))</f>
         <v/>
       </c>
       <c r="AY10" s="78" t="s">
@@ -4585,7 +4604,7 @@
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
       <c r="O11" s="35">
-        <f>SUM(C11:N11)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P11" s="36">
@@ -4593,7 +4612,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="36">
-        <f>COUNT(C11:N11)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R11" s="45"/>
@@ -4692,27 +4711,27 @@
         <v>0</v>
       </c>
       <c r="AS11" s="77" t="str">
-        <f>IF(S11="","",IF(C11=0,0,1+2*S11))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT11" s="78" t="str">
-        <f>IF(T11="","",IF(D11=0,0,1+2*T11))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU11" s="78" t="str">
-        <f>IF(U11="","",IF(E11=0,0,1+2*U11))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV11" s="78" t="str">
-        <f>IF(V11="","",IF(F11=0,0,1+2*V11))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AW11" s="78" t="str">
-        <f>IF(W11="","",IF(G11=0,0,1+2*W11))</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AX11" s="78" t="str">
-        <f>IF(X11="","",IF(H11=0,0,1+2*X11))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AY11" s="78" t="str">
@@ -4759,7 +4778,7 @@
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
       <c r="O12" s="35">
-        <f>SUM(C12:N12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P12" s="36">
@@ -4767,7 +4786,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="36">
-        <f>COUNT(C12:N12)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R12" s="45"/>
@@ -4866,27 +4885,27 @@
         <v>0</v>
       </c>
       <c r="AS12" s="77" t="str">
-        <f>IF(S12="","",IF(C12=0,0,1+2*S12))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT12" s="78" t="str">
-        <f>IF(T12="","",IF(D12=0,0,1+2*T12))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU12" s="78" t="str">
-        <f>IF(U12="","",IF(E12=0,0,1+2*U12))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV12" s="78" t="str">
-        <f>IF(V12="","",IF(F12=0,0,1+2*V12))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AW12" s="78" t="str">
-        <f>IF(W12="","",IF(G12=0,0,1+2*W12))</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AX12" s="78" t="str">
-        <f>IF(X12="","",IF(H12=0,0,1+2*X12))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AY12" s="78" t="str">
@@ -4933,7 +4952,7 @@
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
       <c r="O13" s="35">
-        <f>SUM(C13:N13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P13" s="36">
@@ -4941,7 +4960,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="36">
-        <f>COUNT(C13:N13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R13" s="45"/>
@@ -5040,27 +5059,27 @@
         <v>0</v>
       </c>
       <c r="AS13" s="77" t="str">
-        <f>IF(S13="","",IF(C13=0,0,1+2*S13))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT13" s="78" t="str">
-        <f>IF(T13="","",IF(D13=0,0,1+2*T13))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU13" s="78" t="str">
-        <f>IF(U13="","",IF(E13=0,0,1+2*U13))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV13" s="78" t="str">
-        <f>IF(V13="","",IF(F13=0,0,1+2*V13))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AW13" s="78" t="str">
-        <f>IF(W13="","",IF(G13=0,0,1+2*W13))</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AX13" s="78" t="str">
-        <f>IF(X13="","",IF(H13=0,0,1+2*X13))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AY13" s="78" t="str">
@@ -5107,7 +5126,7 @@
       </c>
       <c r="N14" s="34"/>
       <c r="O14" s="35">
-        <f>SUM(C14:N14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P14" s="36">
@@ -5115,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="36">
-        <f>COUNT(C14:N14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R14" s="45"/>
@@ -5214,27 +5233,27 @@
         <v>0</v>
       </c>
       <c r="AS14" s="77" t="str">
-        <f>IF(S14="","",IF(C14=0,0,1+2*S14))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT14" s="78" t="str">
-        <f>IF(T14="","",IF(D14=0,0,1+2*T14))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU14" s="78" t="str">
-        <f>IF(U14="","",IF(E14=0,0,1+2*U14))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV14" s="78" t="str">
-        <f>IF(V14="","",IF(F14=0,0,1+2*V14))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AW14" s="78" t="str">
-        <f>IF(W14="","",IF(G14=0,0,1+2*W14))</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AX14" s="78" t="str">
-        <f>IF(X14="","",IF(H14=0,0,1+2*X14))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AY14" s="78" t="str">
@@ -5281,7 +5300,7 @@
         <v>37</v>
       </c>
       <c r="O15" s="41">
-        <f>SUM(C15:N15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="P15" s="42">
@@ -5289,7 +5308,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="42">
-        <f>COUNT(C15:N15)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R15" s="45"/>
@@ -5388,27 +5407,27 @@
         <v>37</v>
       </c>
       <c r="AS15" s="80" t="str">
-        <f>IF(S15="","",IF(C15=0,0,1+2*S15))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AT15" s="81" t="str">
-        <f>IF(T15="","",IF(D15=0,0,1+2*T15))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AU15" s="81" t="str">
-        <f>IF(U15="","",IF(E15=0,0,1+2*U15))</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AV15" s="81" t="str">
-        <f>IF(V15="","",IF(F15=0,0,1+2*V15))</f>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="AW15" s="81" t="str">
-        <f>IF(W15="","",IF(G15=0,0,1+2*W15))</f>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AX15" s="81" t="str">
-        <f>IF(X15="","",IF(H15=0,0,1+2*X15))</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="AY15" s="81" t="str">
@@ -5460,51 +5479,51 @@
         <v>33</v>
       </c>
       <c r="C17" s="28">
-        <f>MATCH("XX",C18:C29,0)</f>
+        <f t="shared" ref="C17:N17" si="15">MATCH("XX",C18:C29,0)</f>
         <v>1</v>
       </c>
       <c r="D17" s="28">
-        <f>MATCH("XX",D18:D29,0)</f>
+        <f t="shared" si="15"/>
         <v>2</v>
       </c>
       <c r="E17" s="28">
-        <f>MATCH("XX",E18:E29,0)</f>
+        <f t="shared" si="15"/>
         <v>3</v>
       </c>
       <c r="F17" s="28">
-        <f>MATCH("XX",F18:F29,0)</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="G17" s="28">
-        <f>MATCH("XX",G18:G29,0)</f>
+        <f t="shared" si="15"/>
         <v>5</v>
       </c>
       <c r="H17" s="28">
-        <f>MATCH("XX",H18:H29,0)</f>
+        <f t="shared" si="15"/>
         <v>6</v>
       </c>
       <c r="I17" s="28">
-        <f>MATCH("XX",I18:I29,0)</f>
+        <f t="shared" si="15"/>
         <v>7</v>
       </c>
       <c r="J17" s="28">
-        <f>MATCH("XX",J18:J29,0)</f>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="K17" s="28">
-        <f>MATCH("XX",K18:K29,0)</f>
+        <f t="shared" si="15"/>
         <v>9</v>
       </c>
       <c r="L17" s="28">
-        <f>MATCH("XX",L18:L29,0)</f>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="M17" s="28">
-        <f>MATCH("XX",M18:M29,0)</f>
+        <f t="shared" si="15"/>
         <v>11</v>
       </c>
       <c r="N17" s="28">
-        <f>MATCH("XX",N18:N29,0)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="O17" s="29" t="s">
@@ -5549,7 +5568,7 @@
       <c r="M18" s="34"/>
       <c r="N18" s="34"/>
       <c r="O18" s="35">
-        <f>SUM(C18:N18)</f>
+        <f t="shared" ref="O18:O29" si="16">SUM(C18:N18)</f>
         <v>0</v>
       </c>
       <c r="P18" s="36">
@@ -5557,7 +5576,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="36">
-        <f>COUNT(C18:N18)</f>
+        <f t="shared" ref="Q18:Q29" si="17">COUNT(C18:N18)</f>
         <v>0</v>
       </c>
       <c r="R18" s="45"/>
@@ -5659,47 +5678,47 @@
         <v>37</v>
       </c>
       <c r="AT18" s="75" t="str">
-        <f>IF(T18="","",IF(D18=0,0,1+2*T18))</f>
+        <f t="shared" ref="AT18:BD18" si="18">IF(T18="","",IF(D18=0,0,1+2*T18))</f>
         <v/>
       </c>
       <c r="AU18" s="75" t="str">
-        <f>IF(U18="","",IF(E18=0,0,1+2*U18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AV18" s="75" t="str">
-        <f>IF(V18="","",IF(F18=0,0,1+2*V18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AW18" s="75" t="str">
-        <f>IF(W18="","",IF(G18=0,0,1+2*W18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AX18" s="75" t="str">
-        <f>IF(X18="","",IF(H18=0,0,1+2*X18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AY18" s="75" t="str">
-        <f>IF(Y18="","",IF(I18=0,0,1+2*Y18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="AZ18" s="75" t="str">
-        <f>IF(Z18="","",IF(J18=0,0,1+2*Z18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="BA18" s="75" t="str">
-        <f>IF(AA18="","",IF(K18=0,0,1+2*AA18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="BB18" s="75" t="str">
-        <f>IF(AB18="","",IF(L18=0,0,1+2*AB18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="BC18" s="75" t="str">
-        <f>IF(AC18="","",IF(M18=0,0,1+2*AC18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="BD18" s="76" t="str">
-        <f>IF(AD18="","",IF(N18=0,0,1+2*AD18))</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
     </row>
@@ -5723,7 +5742,7 @@
       <c r="M19" s="34"/>
       <c r="N19" s="34"/>
       <c r="O19" s="35">
-        <f>SUM(C19:N19)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P19" s="36">
@@ -5731,7 +5750,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="36">
-        <f>COUNT(C19:N19)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R19" s="45"/>
@@ -5830,50 +5849,50 @@
         <v>0</v>
       </c>
       <c r="AS19" s="77" t="str">
-        <f>IF(S19="","",IF(C19=0,0,1+2*S19))</f>
+        <f t="shared" ref="AS19:AS29" si="19">IF(S19="","",IF(C19=0,0,1+2*S19))</f>
         <v/>
       </c>
       <c r="AT19" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AU19" s="78" t="str">
-        <f>IF(U19="","",IF(E19=0,0,1+2*U19))</f>
+        <f t="shared" ref="AU19:BD19" si="20">IF(U19="","",IF(E19=0,0,1+2*U19))</f>
         <v/>
       </c>
       <c r="AV19" s="78" t="str">
-        <f>IF(V19="","",IF(F19=0,0,1+2*V19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AW19" s="78" t="str">
-        <f>IF(W19="","",IF(G19=0,0,1+2*W19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AX19" s="78" t="str">
-        <f>IF(X19="","",IF(H19=0,0,1+2*X19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AY19" s="78" t="str">
-        <f>IF(Y19="","",IF(I19=0,0,1+2*Y19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AZ19" s="78" t="str">
-        <f>IF(Z19="","",IF(J19=0,0,1+2*Z19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="BA19" s="78" t="str">
-        <f>IF(AA19="","",IF(K19=0,0,1+2*AA19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="BB19" s="78" t="str">
-        <f>IF(AB19="","",IF(L19=0,0,1+2*AB19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="BC19" s="78" t="str">
-        <f>IF(AC19="","",IF(M19=0,0,1+2*AC19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="BD19" s="79" t="str">
-        <f>IF(AD19="","",IF(N19=0,0,1+2*AD19))</f>
+        <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
@@ -5897,7 +5916,7 @@
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
       <c r="O20" s="35">
-        <f>SUM(C20:N20)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P20" s="36">
@@ -5905,7 +5924,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="36">
-        <f>COUNT(C20:N20)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R20" s="45"/>
@@ -6004,50 +6023,50 @@
         <v>0</v>
       </c>
       <c r="AS20" s="77" t="str">
-        <f>IF(S20="","",IF(C20=0,0,1+2*S20))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT20" s="78" t="str">
-        <f>IF(T20="","",IF(D20=0,0,1+2*T20))</f>
+        <f t="shared" ref="AT20:AT29" si="21">IF(T20="","",IF(D20=0,0,1+2*T20))</f>
         <v/>
       </c>
       <c r="AU20" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AV20" s="78" t="str">
-        <f>IF(V20="","",IF(F20=0,0,1+2*V20))</f>
+        <f t="shared" ref="AV20:BD20" si="22">IF(V20="","",IF(F20=0,0,1+2*V20))</f>
         <v/>
       </c>
       <c r="AW20" s="78" t="str">
-        <f>IF(W20="","",IF(G20=0,0,1+2*W20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="AX20" s="78" t="str">
-        <f>IF(X20="","",IF(H20=0,0,1+2*X20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="AY20" s="78" t="str">
-        <f>IF(Y20="","",IF(I20=0,0,1+2*Y20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="AZ20" s="78" t="str">
-        <f>IF(Z20="","",IF(J20=0,0,1+2*Z20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="BA20" s="78" t="str">
-        <f>IF(AA20="","",IF(K20=0,0,1+2*AA20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="BB20" s="78" t="str">
-        <f>IF(AB20="","",IF(L20=0,0,1+2*AB20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="BC20" s="78" t="str">
-        <f>IF(AC20="","",IF(M20=0,0,1+2*AC20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="BD20" s="79" t="str">
-        <f>IF(AD20="","",IF(N20=0,0,1+2*AD20))</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
     </row>
@@ -6071,7 +6090,7 @@
       <c r="M21" s="34"/>
       <c r="N21" s="34"/>
       <c r="O21" s="35">
-        <f>SUM(C21:N21)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P21" s="36">
@@ -6079,7 +6098,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="36">
-        <f>COUNT(C21:N21)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R21" s="45"/>
@@ -6178,50 +6197,50 @@
         <v>0</v>
       </c>
       <c r="AS21" s="77" t="str">
-        <f>IF(S21="","",IF(C21=0,0,1+2*S21))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT21" s="78" t="str">
-        <f>IF(T21="","",IF(D21=0,0,1+2*T21))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU21" s="78" t="str">
-        <f>IF(U21="","",IF(E21=0,0,1+2*U21))</f>
+        <f t="shared" ref="AU21:AU29" si="23">IF(U21="","",IF(E21=0,0,1+2*U21))</f>
         <v/>
       </c>
       <c r="AV21" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AW21" s="78" t="str">
-        <f>IF(W21="","",IF(G21=0,0,1+2*W21))</f>
+        <f t="shared" ref="AW21:BD21" si="24">IF(W21="","",IF(G21=0,0,1+2*W21))</f>
         <v/>
       </c>
       <c r="AX21" s="78" t="str">
-        <f>IF(X21="","",IF(H21=0,0,1+2*X21))</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AY21" s="78" t="str">
-        <f>IF(Y21="","",IF(I21=0,0,1+2*Y21))</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="AZ21" s="78" t="str">
-        <f>IF(Z21="","",IF(J21=0,0,1+2*Z21))</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="BA21" s="78" t="str">
-        <f>IF(AA21="","",IF(K21=0,0,1+2*AA21))</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="BB21" s="78" t="str">
-        <f>IF(AB21="","",IF(L21=0,0,1+2*AB21))</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="BC21" s="78" t="str">
-        <f>IF(AC21="","",IF(M21=0,0,1+2*AC21))</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="BD21" s="79" t="str">
-        <f>IF(AD21="","",IF(N21=0,0,1+2*AD21))</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
     </row>
@@ -6245,7 +6264,7 @@
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
       <c r="O22" s="35">
-        <f>SUM(C22:N22)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P22" s="36">
@@ -6253,7 +6272,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="36">
-        <f>COUNT(C22:N22)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R22" s="45"/>
@@ -6352,50 +6371,50 @@
         <v>0</v>
       </c>
       <c r="AS22" s="77" t="str">
-        <f>IF(S22="","",IF(C22=0,0,1+2*S22))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT22" s="78" t="str">
-        <f>IF(T22="","",IF(D22=0,0,1+2*T22))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU22" s="78" t="str">
-        <f>IF(U22="","",IF(E22=0,0,1+2*U22))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV22" s="78" t="str">
-        <f>IF(V22="","",IF(F22=0,0,1+2*V22))</f>
+        <f t="shared" ref="AV22:AV29" si="25">IF(V22="","",IF(F22=0,0,1+2*V22))</f>
         <v/>
       </c>
       <c r="AW22" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AX22" s="78" t="str">
-        <f>IF(X22="","",IF(H22=0,0,1+2*X22))</f>
+        <f t="shared" ref="AX22:BD22" si="26">IF(X22="","",IF(H22=0,0,1+2*X22))</f>
         <v/>
       </c>
       <c r="AY22" s="78" t="str">
-        <f>IF(Y22="","",IF(I22=0,0,1+2*Y22))</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="AZ22" s="78" t="str">
-        <f>IF(Z22="","",IF(J22=0,0,1+2*Z22))</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="BA22" s="78" t="str">
-        <f>IF(AA22="","",IF(K22=0,0,1+2*AA22))</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="BB22" s="78" t="str">
-        <f>IF(AB22="","",IF(L22=0,0,1+2*AB22))</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="BC22" s="78" t="str">
-        <f>IF(AC22="","",IF(M22=0,0,1+2*AC22))</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
       <c r="BD22" s="79" t="str">
-        <f>IF(AD22="","",IF(N22=0,0,1+2*AD22))</f>
+        <f t="shared" si="26"/>
         <v/>
       </c>
     </row>
@@ -6419,7 +6438,7 @@
       <c r="M23" s="34"/>
       <c r="N23" s="34"/>
       <c r="O23" s="35">
-        <f>SUM(C23:N23)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P23" s="36">
@@ -6427,7 +6446,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="36">
-        <f>COUNT(C23:N23)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R23" s="45"/>
@@ -6526,50 +6545,50 @@
         <v>0</v>
       </c>
       <c r="AS23" s="77" t="str">
-        <f>IF(S23="","",IF(C23=0,0,1+2*S23))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT23" s="78" t="str">
-        <f>IF(T23="","",IF(D23=0,0,1+2*T23))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU23" s="78" t="str">
-        <f>IF(U23="","",IF(E23=0,0,1+2*U23))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV23" s="78" t="str">
-        <f>IF(V23="","",IF(F23=0,0,1+2*V23))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AW23" s="78" t="str">
-        <f>IF(W23="","",IF(G23=0,0,1+2*W23))</f>
+        <f t="shared" ref="AW23:AW29" si="27">IF(W23="","",IF(G23=0,0,1+2*W23))</f>
         <v/>
       </c>
       <c r="AX23" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AY23" s="78" t="str">
-        <f>IF(Y23="","",IF(I23=0,0,1+2*Y23))</f>
+        <f t="shared" ref="AY23:BD23" si="28">IF(Y23="","",IF(I23=0,0,1+2*Y23))</f>
         <v/>
       </c>
       <c r="AZ23" s="78" t="str">
-        <f>IF(Z23="","",IF(J23=0,0,1+2*Z23))</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="BA23" s="78" t="str">
-        <f>IF(AA23="","",IF(K23=0,0,1+2*AA23))</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="BB23" s="78" t="str">
-        <f>IF(AB23="","",IF(L23=0,0,1+2*AB23))</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="BC23" s="78" t="str">
-        <f>IF(AC23="","",IF(M23=0,0,1+2*AC23))</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
       <c r="BD23" s="79" t="str">
-        <f>IF(AD23="","",IF(N23=0,0,1+2*AD23))</f>
+        <f t="shared" si="28"/>
         <v/>
       </c>
     </row>
@@ -6593,7 +6612,7 @@
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
       <c r="O24" s="35">
-        <f>SUM(C24:N24)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P24" s="36">
@@ -6601,7 +6620,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="36">
-        <f>COUNT(C24:N24)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R24" s="45"/>
@@ -6700,27 +6719,27 @@
         <v>0</v>
       </c>
       <c r="AS24" s="77" t="str">
-        <f>IF(S24="","",IF(C24=0,0,1+2*S24))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT24" s="78" t="str">
-        <f>IF(T24="","",IF(D24=0,0,1+2*T24))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU24" s="78" t="str">
-        <f>IF(U24="","",IF(E24=0,0,1+2*U24))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV24" s="78" t="str">
-        <f>IF(V24="","",IF(F24=0,0,1+2*V24))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AW24" s="78" t="str">
-        <f>IF(W24="","",IF(G24=0,0,1+2*W24))</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AX24" s="78" t="str">
-        <f>IF(X24="","",IF(H24=0,0,1+2*X24))</f>
+        <f t="shared" ref="AX24:AX29" si="29">IF(X24="","",IF(H24=0,0,1+2*X24))</f>
         <v/>
       </c>
       <c r="AY24" s="78" t="s">
@@ -6767,7 +6786,7 @@
       <c r="M25" s="34"/>
       <c r="N25" s="34"/>
       <c r="O25" s="35">
-        <f>SUM(C25:N25)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P25" s="36">
@@ -6775,7 +6794,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="36">
-        <f>COUNT(C25:N25)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R25" s="45"/>
@@ -6874,27 +6893,27 @@
         <v>0</v>
       </c>
       <c r="AS25" s="77" t="str">
-        <f>IF(S25="","",IF(C25=0,0,1+2*S25))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT25" s="78" t="str">
-        <f>IF(T25="","",IF(D25=0,0,1+2*T25))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU25" s="78" t="str">
-        <f>IF(U25="","",IF(E25=0,0,1+2*U25))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV25" s="78" t="str">
-        <f>IF(V25="","",IF(F25=0,0,1+2*V25))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AW25" s="78" t="str">
-        <f>IF(W25="","",IF(G25=0,0,1+2*W25))</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AX25" s="78" t="str">
-        <f>IF(X25="","",IF(H25=0,0,1+2*X25))</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AY25" s="78" t="str">
@@ -6941,7 +6960,7 @@
       <c r="M26" s="34"/>
       <c r="N26" s="34"/>
       <c r="O26" s="35">
-        <f>SUM(C26:N26)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P26" s="36">
@@ -6949,7 +6968,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="36">
-        <f>COUNT(C26:N26)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R26" s="45"/>
@@ -7048,27 +7067,27 @@
         <v>0</v>
       </c>
       <c r="AS26" s="77" t="str">
-        <f>IF(S26="","",IF(C26=0,0,1+2*S26))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT26" s="78" t="str">
-        <f>IF(T26="","",IF(D26=0,0,1+2*T26))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU26" s="78" t="str">
-        <f>IF(U26="","",IF(E26=0,0,1+2*U26))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV26" s="78" t="str">
-        <f>IF(V26="","",IF(F26=0,0,1+2*V26))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AW26" s="78" t="str">
-        <f>IF(W26="","",IF(G26=0,0,1+2*W26))</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AX26" s="78" t="str">
-        <f>IF(X26="","",IF(H26=0,0,1+2*X26))</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AY26" s="78" t="str">
@@ -7115,7 +7134,7 @@
       <c r="M27" s="34"/>
       <c r="N27" s="34"/>
       <c r="O27" s="35">
-        <f>SUM(C27:N27)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P27" s="36">
@@ -7123,7 +7142,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="36">
-        <f>COUNT(C27:N27)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R27" s="45"/>
@@ -7222,27 +7241,27 @@
         <v>0</v>
       </c>
       <c r="AS27" s="77" t="str">
-        <f>IF(S27="","",IF(C27=0,0,1+2*S27))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT27" s="78" t="str">
-        <f>IF(T27="","",IF(D27=0,0,1+2*T27))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU27" s="78" t="str">
-        <f>IF(U27="","",IF(E27=0,0,1+2*U27))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV27" s="78" t="str">
-        <f>IF(V27="","",IF(F27=0,0,1+2*V27))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AW27" s="78" t="str">
-        <f>IF(W27="","",IF(G27=0,0,1+2*W27))</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AX27" s="78" t="str">
-        <f>IF(X27="","",IF(H27=0,0,1+2*X27))</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AY27" s="78" t="str">
@@ -7289,7 +7308,7 @@
       </c>
       <c r="N28" s="34"/>
       <c r="O28" s="35">
-        <f>SUM(C28:N28)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P28" s="36">
@@ -7297,7 +7316,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="36">
-        <f>COUNT(C28:N28)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R28" s="45"/>
@@ -7396,27 +7415,27 @@
         <v>0</v>
       </c>
       <c r="AS28" s="77" t="str">
-        <f>IF(S28="","",IF(C28=0,0,1+2*S28))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT28" s="78" t="str">
-        <f>IF(T28="","",IF(D28=0,0,1+2*T28))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU28" s="78" t="str">
-        <f>IF(U28="","",IF(E28=0,0,1+2*U28))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV28" s="78" t="str">
-        <f>IF(V28="","",IF(F28=0,0,1+2*V28))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AW28" s="78" t="str">
-        <f>IF(W28="","",IF(G28=0,0,1+2*W28))</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AX28" s="78" t="str">
-        <f>IF(X28="","",IF(H28=0,0,1+2*X28))</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AY28" s="78" t="str">
@@ -7463,7 +7482,7 @@
         <v>37</v>
       </c>
       <c r="O29" s="41">
-        <f>SUM(C29:N29)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P29" s="42">
@@ -7471,7 +7490,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="42">
-        <f>COUNT(C29:N29)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R29" s="45"/>
@@ -7570,27 +7589,27 @@
         <v>37</v>
       </c>
       <c r="AS29" s="80" t="str">
-        <f>IF(S29="","",IF(C29=0,0,1+2*S29))</f>
+        <f t="shared" si="19"/>
         <v/>
       </c>
       <c r="AT29" s="81" t="str">
-        <f>IF(T29="","",IF(D29=0,0,1+2*T29))</f>
+        <f t="shared" si="21"/>
         <v/>
       </c>
       <c r="AU29" s="81" t="str">
-        <f>IF(U29="","",IF(E29=0,0,1+2*U29))</f>
+        <f t="shared" si="23"/>
         <v/>
       </c>
       <c r="AV29" s="81" t="str">
-        <f>IF(V29="","",IF(F29=0,0,1+2*V29))</f>
+        <f t="shared" si="25"/>
         <v/>
       </c>
       <c r="AW29" s="81" t="str">
-        <f>IF(W29="","",IF(G29=0,0,1+2*W29))</f>
+        <f t="shared" si="27"/>
         <v/>
       </c>
       <c r="AX29" s="81" t="str">
-        <f>IF(X29="","",IF(H29=0,0,1+2*X29))</f>
+        <f t="shared" si="29"/>
         <v/>
       </c>
       <c r="AY29" s="81" t="str">
@@ -7642,51 +7661,51 @@
         <v>33</v>
       </c>
       <c r="C31" s="28">
-        <f>MATCH("XX",C32:C43,0)</f>
+        <f t="shared" ref="C31:N31" si="30">MATCH("XX",C32:C43,0)</f>
         <v>1</v>
       </c>
       <c r="D31" s="28">
-        <f>MATCH("XX",D32:D43,0)</f>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="E31" s="28">
-        <f>MATCH("XX",E32:E43,0)</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="F31" s="28">
-        <f>MATCH("XX",F32:F43,0)</f>
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
       <c r="G31" s="28">
-        <f>MATCH("XX",G32:G43,0)</f>
+        <f t="shared" si="30"/>
         <v>5</v>
       </c>
       <c r="H31" s="28">
-        <f>MATCH("XX",H32:H43,0)</f>
+        <f t="shared" si="30"/>
         <v>6</v>
       </c>
       <c r="I31" s="28">
-        <f>MATCH("XX",I32:I43,0)</f>
+        <f t="shared" si="30"/>
         <v>7</v>
       </c>
       <c r="J31" s="28">
-        <f>MATCH("XX",J32:J43,0)</f>
+        <f t="shared" si="30"/>
         <v>8</v>
       </c>
       <c r="K31" s="28">
-        <f>MATCH("XX",K32:K43,0)</f>
+        <f t="shared" si="30"/>
         <v>9</v>
       </c>
       <c r="L31" s="28">
-        <f>MATCH("XX",L32:L43,0)</f>
+        <f t="shared" si="30"/>
         <v>10</v>
       </c>
       <c r="M31" s="28">
-        <f>MATCH("XX",M32:M43,0)</f>
+        <f t="shared" si="30"/>
         <v>11</v>
       </c>
       <c r="N31" s="28">
-        <f>MATCH("XX",N32:N43,0)</f>
+        <f t="shared" si="30"/>
         <v>12</v>
       </c>
       <c r="O31" s="29" t="s">
@@ -7731,7 +7750,7 @@
       <c r="M32" s="34"/>
       <c r="N32" s="34"/>
       <c r="O32" s="35">
-        <f>SUM(C32:N32)</f>
+        <f t="shared" ref="O32:O43" si="31">SUM(C32:N32)</f>
         <v>0</v>
       </c>
       <c r="P32" s="36">
@@ -7739,7 +7758,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="36">
-        <f>COUNT(C32:N32)</f>
+        <f t="shared" ref="Q32:Q43" si="32">COUNT(C32:N32)</f>
         <v>0</v>
       </c>
       <c r="R32" s="45"/>
@@ -7841,47 +7860,47 @@
         <v>37</v>
       </c>
       <c r="AT32" s="75" t="str">
-        <f>IF(T32="","",IF(D32=0,0,1+2*T32))</f>
+        <f t="shared" ref="AT32:BD32" si="33">IF(T32="","",IF(D32=0,0,1+2*T32))</f>
         <v/>
       </c>
       <c r="AU32" s="75" t="str">
-        <f>IF(U32="","",IF(E32=0,0,1+2*U32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AV32" s="75" t="str">
-        <f>IF(V32="","",IF(F32=0,0,1+2*V32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AW32" s="75" t="str">
-        <f>IF(W32="","",IF(G32=0,0,1+2*W32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AX32" s="75" t="str">
-        <f>IF(X32="","",IF(H32=0,0,1+2*X32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AY32" s="75" t="str">
-        <f>IF(Y32="","",IF(I32=0,0,1+2*Y32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="AZ32" s="75" t="str">
-        <f>IF(Z32="","",IF(J32=0,0,1+2*Z32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="BA32" s="75" t="str">
-        <f>IF(AA32="","",IF(K32=0,0,1+2*AA32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="BB32" s="75" t="str">
-        <f>IF(AB32="","",IF(L32=0,0,1+2*AB32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="BC32" s="75" t="str">
-        <f>IF(AC32="","",IF(M32=0,0,1+2*AC32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
       <c r="BD32" s="76" t="str">
-        <f>IF(AD32="","",IF(N32=0,0,1+2*AD32))</f>
+        <f t="shared" si="33"/>
         <v/>
       </c>
     </row>
@@ -7905,7 +7924,7 @@
       <c r="M33" s="34"/>
       <c r="N33" s="34"/>
       <c r="O33" s="35">
-        <f>SUM(C33:N33)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P33" s="36">
@@ -7913,7 +7932,7 @@
         <v>0</v>
       </c>
       <c r="Q33" s="36">
-        <f>COUNT(C33:N33)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R33" s="45"/>
@@ -8012,50 +8031,50 @@
         <v>0</v>
       </c>
       <c r="AS33" s="77" t="str">
-        <f>IF(S33="","",IF(C33=0,0,1+2*S33))</f>
+        <f t="shared" ref="AS33:AS43" si="34">IF(S33="","",IF(C33=0,0,1+2*S33))</f>
         <v/>
       </c>
       <c r="AT33" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AU33" s="78" t="str">
-        <f>IF(U33="","",IF(E33=0,0,1+2*U33))</f>
+        <f t="shared" ref="AU33:BD33" si="35">IF(U33="","",IF(E33=0,0,1+2*U33))</f>
         <v/>
       </c>
       <c r="AV33" s="78" t="str">
-        <f>IF(V33="","",IF(F33=0,0,1+2*V33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AW33" s="78" t="str">
-        <f>IF(W33="","",IF(G33=0,0,1+2*W33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AX33" s="78" t="str">
-        <f>IF(X33="","",IF(H33=0,0,1+2*X33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AY33" s="78" t="str">
-        <f>IF(Y33="","",IF(I33=0,0,1+2*Y33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="AZ33" s="78" t="str">
-        <f>IF(Z33="","",IF(J33=0,0,1+2*Z33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="BA33" s="78" t="str">
-        <f>IF(AA33="","",IF(K33=0,0,1+2*AA33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="BB33" s="78" t="str">
-        <f>IF(AB33="","",IF(L33=0,0,1+2*AB33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="BC33" s="78" t="str">
-        <f>IF(AC33="","",IF(M33=0,0,1+2*AC33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
       <c r="BD33" s="79" t="str">
-        <f>IF(AD33="","",IF(N33=0,0,1+2*AD33))</f>
+        <f t="shared" si="35"/>
         <v/>
       </c>
     </row>
@@ -8079,7 +8098,7 @@
       <c r="M34" s="34"/>
       <c r="N34" s="34"/>
       <c r="O34" s="35">
-        <f>SUM(C34:N34)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P34" s="36">
@@ -8087,7 +8106,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="36">
-        <f>COUNT(C34:N34)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R34" s="45"/>
@@ -8186,50 +8205,50 @@
         <v>0</v>
       </c>
       <c r="AS34" s="77" t="str">
-        <f>IF(S34="","",IF(C34=0,0,1+2*S34))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT34" s="78" t="str">
-        <f>IF(T34="","",IF(D34=0,0,1+2*T34))</f>
+        <f t="shared" ref="AT34:AT43" si="36">IF(T34="","",IF(D34=0,0,1+2*T34))</f>
         <v/>
       </c>
       <c r="AU34" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AV34" s="78" t="str">
-        <f>IF(V34="","",IF(F34=0,0,1+2*V34))</f>
+        <f t="shared" ref="AV34:BD34" si="37">IF(V34="","",IF(F34=0,0,1+2*V34))</f>
         <v/>
       </c>
       <c r="AW34" s="78" t="str">
-        <f>IF(W34="","",IF(G34=0,0,1+2*W34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="AX34" s="78" t="str">
-        <f>IF(X34="","",IF(H34=0,0,1+2*X34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="AY34" s="78" t="str">
-        <f>IF(Y34="","",IF(I34=0,0,1+2*Y34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="AZ34" s="78" t="str">
-        <f>IF(Z34="","",IF(J34=0,0,1+2*Z34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="BA34" s="78" t="str">
-        <f>IF(AA34="","",IF(K34=0,0,1+2*AA34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="BB34" s="78" t="str">
-        <f>IF(AB34="","",IF(L34=0,0,1+2*AB34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="BC34" s="78" t="str">
-        <f>IF(AC34="","",IF(M34=0,0,1+2*AC34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
       <c r="BD34" s="79" t="str">
-        <f>IF(AD34="","",IF(N34=0,0,1+2*AD34))</f>
+        <f t="shared" si="37"/>
         <v/>
       </c>
     </row>
@@ -8253,7 +8272,7 @@
       <c r="M35" s="34"/>
       <c r="N35" s="34"/>
       <c r="O35" s="35">
-        <f>SUM(C35:N35)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P35" s="36">
@@ -8261,7 +8280,7 @@
         <v>0</v>
       </c>
       <c r="Q35" s="36">
-        <f>COUNT(C35:N35)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R35" s="45"/>
@@ -8360,50 +8379,50 @@
         <v>0</v>
       </c>
       <c r="AS35" s="77" t="str">
-        <f>IF(S35="","",IF(C35=0,0,1+2*S35))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT35" s="78" t="str">
-        <f>IF(T35="","",IF(D35=0,0,1+2*T35))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU35" s="78" t="str">
-        <f>IF(U35="","",IF(E35=0,0,1+2*U35))</f>
+        <f t="shared" ref="AU35:AU43" si="38">IF(U35="","",IF(E35=0,0,1+2*U35))</f>
         <v/>
       </c>
       <c r="AV35" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AW35" s="78" t="str">
-        <f>IF(W35="","",IF(G35=0,0,1+2*W35))</f>
+        <f t="shared" ref="AW35:BD35" si="39">IF(W35="","",IF(G35=0,0,1+2*W35))</f>
         <v/>
       </c>
       <c r="AX35" s="78" t="str">
-        <f>IF(X35="","",IF(H35=0,0,1+2*X35))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="AY35" s="78" t="str">
-        <f>IF(Y35="","",IF(I35=0,0,1+2*Y35))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="AZ35" s="78" t="str">
-        <f>IF(Z35="","",IF(J35=0,0,1+2*Z35))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="BA35" s="78" t="str">
-        <f>IF(AA35="","",IF(K35=0,0,1+2*AA35))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="BB35" s="78" t="str">
-        <f>IF(AB35="","",IF(L35=0,0,1+2*AB35))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="BC35" s="78" t="str">
-        <f>IF(AC35="","",IF(M35=0,0,1+2*AC35))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="BD35" s="79" t="str">
-        <f>IF(AD35="","",IF(N35=0,0,1+2*AD35))</f>
+        <f t="shared" si="39"/>
         <v/>
       </c>
     </row>
@@ -8427,7 +8446,7 @@
       <c r="M36" s="34"/>
       <c r="N36" s="34"/>
       <c r="O36" s="35">
-        <f>SUM(C36:N36)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P36" s="36">
@@ -8435,7 +8454,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="36">
-        <f>COUNT(C36:N36)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R36" s="45"/>
@@ -8534,50 +8553,50 @@
         <v>0</v>
       </c>
       <c r="AS36" s="77" t="str">
-        <f>IF(S36="","",IF(C36=0,0,1+2*S36))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT36" s="78" t="str">
-        <f>IF(T36="","",IF(D36=0,0,1+2*T36))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU36" s="78" t="str">
-        <f>IF(U36="","",IF(E36=0,0,1+2*U36))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV36" s="78" t="str">
-        <f>IF(V36="","",IF(F36=0,0,1+2*V36))</f>
+        <f t="shared" ref="AV36:AV43" si="40">IF(V36="","",IF(F36=0,0,1+2*V36))</f>
         <v/>
       </c>
       <c r="AW36" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AX36" s="78" t="str">
-        <f>IF(X36="","",IF(H36=0,0,1+2*X36))</f>
+        <f t="shared" ref="AX36:BD36" si="41">IF(X36="","",IF(H36=0,0,1+2*X36))</f>
         <v/>
       </c>
       <c r="AY36" s="78" t="str">
-        <f>IF(Y36="","",IF(I36=0,0,1+2*Y36))</f>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="AZ36" s="78" t="str">
-        <f>IF(Z36="","",IF(J36=0,0,1+2*Z36))</f>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="BA36" s="78" t="str">
-        <f>IF(AA36="","",IF(K36=0,0,1+2*AA36))</f>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="BB36" s="78" t="str">
-        <f>IF(AB36="","",IF(L36=0,0,1+2*AB36))</f>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="BC36" s="78" t="str">
-        <f>IF(AC36="","",IF(M36=0,0,1+2*AC36))</f>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="BD36" s="79" t="str">
-        <f>IF(AD36="","",IF(N36=0,0,1+2*AD36))</f>
+        <f t="shared" si="41"/>
         <v/>
       </c>
     </row>
@@ -8601,7 +8620,7 @@
       <c r="M37" s="34"/>
       <c r="N37" s="34"/>
       <c r="O37" s="35">
-        <f>SUM(C37:N37)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P37" s="36">
@@ -8609,7 +8628,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="36">
-        <f>COUNT(C37:N37)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R37" s="45"/>
@@ -8708,50 +8727,50 @@
         <v>0</v>
       </c>
       <c r="AS37" s="77" t="str">
-        <f>IF(S37="","",IF(C37=0,0,1+2*S37))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT37" s="78" t="str">
-        <f>IF(T37="","",IF(D37=0,0,1+2*T37))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU37" s="78" t="str">
-        <f>IF(U37="","",IF(E37=0,0,1+2*U37))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV37" s="78" t="str">
-        <f>IF(V37="","",IF(F37=0,0,1+2*V37))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AW37" s="78" t="str">
-        <f>IF(W37="","",IF(G37=0,0,1+2*W37))</f>
+        <f t="shared" ref="AW37:AW43" si="42">IF(W37="","",IF(G37=0,0,1+2*W37))</f>
         <v/>
       </c>
       <c r="AX37" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AY37" s="78" t="str">
-        <f>IF(Y37="","",IF(I37=0,0,1+2*Y37))</f>
+        <f t="shared" ref="AY37:BD37" si="43">IF(Y37="","",IF(I37=0,0,1+2*Y37))</f>
         <v/>
       </c>
       <c r="AZ37" s="78" t="str">
-        <f>IF(Z37="","",IF(J37=0,0,1+2*Z37))</f>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="BA37" s="78" t="str">
-        <f>IF(AA37="","",IF(K37=0,0,1+2*AA37))</f>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="BB37" s="78" t="str">
-        <f>IF(AB37="","",IF(L37=0,0,1+2*AB37))</f>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="BC37" s="78" t="str">
-        <f>IF(AC37="","",IF(M37=0,0,1+2*AC37))</f>
+        <f t="shared" si="43"/>
         <v/>
       </c>
       <c r="BD37" s="79" t="str">
-        <f>IF(AD37="","",IF(N37=0,0,1+2*AD37))</f>
+        <f t="shared" si="43"/>
         <v/>
       </c>
     </row>
@@ -8775,7 +8794,7 @@
       <c r="M38" s="34"/>
       <c r="N38" s="34"/>
       <c r="O38" s="35">
-        <f>SUM(C38:N38)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P38" s="36">
@@ -8783,7 +8802,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="36">
-        <f>COUNT(C38:N38)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R38" s="45"/>
@@ -8882,27 +8901,27 @@
         <v>0</v>
       </c>
       <c r="AS38" s="77" t="str">
-        <f>IF(S38="","",IF(C38=0,0,1+2*S38))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT38" s="78" t="str">
-        <f>IF(T38="","",IF(D38=0,0,1+2*T38))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU38" s="78" t="str">
-        <f>IF(U38="","",IF(E38=0,0,1+2*U38))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV38" s="78" t="str">
-        <f>IF(V38="","",IF(F38=0,0,1+2*V38))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AW38" s="78" t="str">
-        <f>IF(W38="","",IF(G38=0,0,1+2*W38))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AX38" s="78" t="str">
-        <f>IF(X38="","",IF(H38=0,0,1+2*X38))</f>
+        <f t="shared" ref="AX38:AX43" si="44">IF(X38="","",IF(H38=0,0,1+2*X38))</f>
         <v/>
       </c>
       <c r="AY38" s="78" t="s">
@@ -8949,7 +8968,7 @@
       <c r="M39" s="34"/>
       <c r="N39" s="34"/>
       <c r="O39" s="35">
-        <f>SUM(C39:N39)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P39" s="36">
@@ -8957,7 +8976,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="36">
-        <f>COUNT(C39:N39)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R39" s="45"/>
@@ -9056,27 +9075,27 @@
         <v>0</v>
       </c>
       <c r="AS39" s="77" t="str">
-        <f>IF(S39="","",IF(C39=0,0,1+2*S39))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT39" s="78" t="str">
-        <f>IF(T39="","",IF(D39=0,0,1+2*T39))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU39" s="78" t="str">
-        <f>IF(U39="","",IF(E39=0,0,1+2*U39))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV39" s="78" t="str">
-        <f>IF(V39="","",IF(F39=0,0,1+2*V39))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AW39" s="78" t="str">
-        <f>IF(W39="","",IF(G39=0,0,1+2*W39))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AX39" s="78" t="str">
-        <f>IF(X39="","",IF(H39=0,0,1+2*X39))</f>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AY39" s="78" t="str">
@@ -9123,7 +9142,7 @@
       <c r="M40" s="34"/>
       <c r="N40" s="34"/>
       <c r="O40" s="35">
-        <f>SUM(C40:N40)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P40" s="36">
@@ -9131,7 +9150,7 @@
         <v>0</v>
       </c>
       <c r="Q40" s="36">
-        <f>COUNT(C40:N40)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R40" s="45"/>
@@ -9230,27 +9249,27 @@
         <v>0</v>
       </c>
       <c r="AS40" s="77" t="str">
-        <f>IF(S40="","",IF(C40=0,0,1+2*S40))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT40" s="78" t="str">
-        <f>IF(T40="","",IF(D40=0,0,1+2*T40))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU40" s="78" t="str">
-        <f>IF(U40="","",IF(E40=0,0,1+2*U40))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV40" s="78" t="str">
-        <f>IF(V40="","",IF(F40=0,0,1+2*V40))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AW40" s="78" t="str">
-        <f>IF(W40="","",IF(G40=0,0,1+2*W40))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AX40" s="78" t="str">
-        <f>IF(X40="","",IF(H40=0,0,1+2*X40))</f>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AY40" s="78" t="str">
@@ -9297,7 +9316,7 @@
       <c r="M41" s="34"/>
       <c r="N41" s="34"/>
       <c r="O41" s="35">
-        <f>SUM(C41:N41)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P41" s="36">
@@ -9305,7 +9324,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="36">
-        <f>COUNT(C41:N41)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R41" s="45"/>
@@ -9404,27 +9423,27 @@
         <v>0</v>
       </c>
       <c r="AS41" s="77" t="str">
-        <f>IF(S41="","",IF(C41=0,0,1+2*S41))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT41" s="78" t="str">
-        <f>IF(T41="","",IF(D41=0,0,1+2*T41))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU41" s="78" t="str">
-        <f>IF(U41="","",IF(E41=0,0,1+2*U41))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV41" s="78" t="str">
-        <f>IF(V41="","",IF(F41=0,0,1+2*V41))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AW41" s="78" t="str">
-        <f>IF(W41="","",IF(G41=0,0,1+2*W41))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AX41" s="78" t="str">
-        <f>IF(X41="","",IF(H41=0,0,1+2*X41))</f>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AY41" s="78" t="str">
@@ -9471,7 +9490,7 @@
       </c>
       <c r="N42" s="34"/>
       <c r="O42" s="35">
-        <f>SUM(C42:N42)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P42" s="36">
@@ -9479,7 +9498,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="36">
-        <f>COUNT(C42:N42)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R42" s="45"/>
@@ -9578,27 +9597,27 @@
         <v>0</v>
       </c>
       <c r="AS42" s="77" t="str">
-        <f>IF(S42="","",IF(C42=0,0,1+2*S42))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT42" s="78" t="str">
-        <f>IF(T42="","",IF(D42=0,0,1+2*T42))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU42" s="78" t="str">
-        <f>IF(U42="","",IF(E42=0,0,1+2*U42))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV42" s="78" t="str">
-        <f>IF(V42="","",IF(F42=0,0,1+2*V42))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AW42" s="78" t="str">
-        <f>IF(W42="","",IF(G42=0,0,1+2*W42))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AX42" s="78" t="str">
-        <f>IF(X42="","",IF(H42=0,0,1+2*X42))</f>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AY42" s="78" t="str">
@@ -9645,7 +9664,7 @@
         <v>37</v>
       </c>
       <c r="O43" s="41">
-        <f>SUM(C43:N43)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="P43" s="42">
@@ -9653,7 +9672,7 @@
         <v>0</v>
       </c>
       <c r="Q43" s="42">
-        <f>COUNT(C43:N43)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="R43" s="45"/>
@@ -9752,27 +9771,27 @@
         <v>37</v>
       </c>
       <c r="AS43" s="80" t="str">
-        <f>IF(S43="","",IF(C43=0,0,1+2*S43))</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="AT43" s="81" t="str">
-        <f>IF(T43="","",IF(D43=0,0,1+2*T43))</f>
+        <f t="shared" si="36"/>
         <v/>
       </c>
       <c r="AU43" s="81" t="str">
-        <f>IF(U43="","",IF(E43=0,0,1+2*U43))</f>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AV43" s="81" t="str">
-        <f>IF(V43="","",IF(F43=0,0,1+2*V43))</f>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="AW43" s="81" t="str">
-        <f>IF(W43="","",IF(G43=0,0,1+2*W43))</f>
+        <f t="shared" si="42"/>
         <v/>
       </c>
       <c r="AX43" s="81" t="str">
-        <f>IF(X43="","",IF(H43=0,0,1+2*X43))</f>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="AY43" s="81" t="str">
@@ -9824,51 +9843,51 @@
         <v>33</v>
       </c>
       <c r="C45" s="28">
-        <f>MATCH("XX",C46:C57,0)</f>
+        <f t="shared" ref="C45:N45" si="45">MATCH("XX",C46:C57,0)</f>
         <v>1</v>
       </c>
       <c r="D45" s="28">
-        <f>MATCH("XX",D46:D57,0)</f>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="E45" s="28">
-        <f>MATCH("XX",E46:E57,0)</f>
+        <f t="shared" si="45"/>
         <v>3</v>
       </c>
       <c r="F45" s="28">
-        <f>MATCH("XX",F46:F57,0)</f>
+        <f t="shared" si="45"/>
         <v>4</v>
       </c>
       <c r="G45" s="28">
-        <f>MATCH("XX",G46:G57,0)</f>
+        <f t="shared" si="45"/>
         <v>5</v>
       </c>
       <c r="H45" s="28">
-        <f>MATCH("XX",H46:H57,0)</f>
+        <f t="shared" si="45"/>
         <v>6</v>
       </c>
       <c r="I45" s="28">
-        <f>MATCH("XX",I46:I57,0)</f>
+        <f t="shared" si="45"/>
         <v>7</v>
       </c>
       <c r="J45" s="28">
-        <f>MATCH("XX",J46:J57,0)</f>
+        <f t="shared" si="45"/>
         <v>8</v>
       </c>
       <c r="K45" s="28">
-        <f>MATCH("XX",K46:K57,0)</f>
+        <f t="shared" si="45"/>
         <v>9</v>
       </c>
       <c r="L45" s="28">
-        <f>MATCH("XX",L46:L57,0)</f>
+        <f t="shared" si="45"/>
         <v>10</v>
       </c>
       <c r="M45" s="28">
-        <f>MATCH("XX",M46:M57,0)</f>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="N45" s="28">
-        <f>MATCH("XX",N46:N57,0)</f>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
       <c r="O45" s="29" t="s">
@@ -9913,7 +9932,7 @@
       <c r="M46" s="34"/>
       <c r="N46" s="34"/>
       <c r="O46" s="35">
-        <f>SUM(C46:N46)</f>
+        <f t="shared" ref="O46:O57" si="46">SUM(C46:N46)</f>
         <v>0</v>
       </c>
       <c r="P46" s="36">
@@ -9921,7 +9940,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="36">
-        <f>COUNT(C46:N46)</f>
+        <f t="shared" ref="Q46:Q57" si="47">COUNT(C46:N46)</f>
         <v>0</v>
       </c>
       <c r="R46" s="45"/>
@@ -10023,47 +10042,47 @@
         <v>37</v>
       </c>
       <c r="AT46" s="75" t="str">
-        <f>IF(T46="","",IF(D46=0,0,1+2*T46))</f>
+        <f t="shared" ref="AT46:BD46" si="48">IF(T46="","",IF(D46=0,0,1+2*T46))</f>
         <v/>
       </c>
       <c r="AU46" s="75" t="str">
-        <f>IF(U46="","",IF(E46=0,0,1+2*U46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AV46" s="75" t="str">
-        <f>IF(V46="","",IF(F46=0,0,1+2*V46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AW46" s="75" t="str">
-        <f>IF(W46="","",IF(G46=0,0,1+2*W46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AX46" s="75" t="str">
-        <f>IF(X46="","",IF(H46=0,0,1+2*X46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AY46" s="75" t="str">
-        <f>IF(Y46="","",IF(I46=0,0,1+2*Y46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="AZ46" s="75" t="str">
-        <f>IF(Z46="","",IF(J46=0,0,1+2*Z46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="BA46" s="75" t="str">
-        <f>IF(AA46="","",IF(K46=0,0,1+2*AA46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="BB46" s="75" t="str">
-        <f>IF(AB46="","",IF(L46=0,0,1+2*AB46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="BC46" s="75" t="str">
-        <f>IF(AC46="","",IF(M46=0,0,1+2*AC46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
       <c r="BD46" s="76" t="str">
-        <f>IF(AD46="","",IF(N46=0,0,1+2*AD46))</f>
+        <f t="shared" si="48"/>
         <v/>
       </c>
     </row>
@@ -10087,7 +10106,7 @@
       <c r="M47" s="34"/>
       <c r="N47" s="34"/>
       <c r="O47" s="35">
-        <f>SUM(C47:N47)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P47" s="36">
@@ -10095,7 +10114,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="36">
-        <f>COUNT(C47:N47)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R47" s="45"/>
@@ -10194,50 +10213,50 @@
         <v>0</v>
       </c>
       <c r="AS47" s="77" t="str">
-        <f>IF(S47="","",IF(C47=0,0,1+2*S47))</f>
+        <f t="shared" ref="AS47:AS57" si="49">IF(S47="","",IF(C47=0,0,1+2*S47))</f>
         <v/>
       </c>
       <c r="AT47" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AU47" s="78" t="str">
-        <f>IF(U47="","",IF(E47=0,0,1+2*U47))</f>
+        <f t="shared" ref="AU47:BD47" si="50">IF(U47="","",IF(E47=0,0,1+2*U47))</f>
         <v/>
       </c>
       <c r="AV47" s="78" t="str">
-        <f>IF(V47="","",IF(F47=0,0,1+2*V47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="AW47" s="78" t="str">
-        <f>IF(W47="","",IF(G47=0,0,1+2*W47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="AX47" s="78" t="str">
-        <f>IF(X47="","",IF(H47=0,0,1+2*X47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="AY47" s="78" t="str">
-        <f>IF(Y47="","",IF(I47=0,0,1+2*Y47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="AZ47" s="78" t="str">
-        <f>IF(Z47="","",IF(J47=0,0,1+2*Z47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="BA47" s="78" t="str">
-        <f>IF(AA47="","",IF(K47=0,0,1+2*AA47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="BB47" s="78" t="str">
-        <f>IF(AB47="","",IF(L47=0,0,1+2*AB47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="BC47" s="78" t="str">
-        <f>IF(AC47="","",IF(M47=0,0,1+2*AC47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="BD47" s="79" t="str">
-        <f>IF(AD47="","",IF(N47=0,0,1+2*AD47))</f>
+        <f t="shared" si="50"/>
         <v/>
       </c>
     </row>
@@ -10261,7 +10280,7 @@
       <c r="M48" s="34"/>
       <c r="N48" s="34"/>
       <c r="O48" s="35">
-        <f>SUM(C48:N48)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P48" s="36">
@@ -10269,7 +10288,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="36">
-        <f>COUNT(C48:N48)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R48" s="45"/>
@@ -10368,50 +10387,50 @@
         <v>0</v>
       </c>
       <c r="AS48" s="77" t="str">
-        <f>IF(S48="","",IF(C48=0,0,1+2*S48))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT48" s="78" t="str">
-        <f>IF(T48="","",IF(D48=0,0,1+2*T48))</f>
+        <f t="shared" ref="AT48:AT57" si="51">IF(T48="","",IF(D48=0,0,1+2*T48))</f>
         <v/>
       </c>
       <c r="AU48" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AV48" s="78" t="str">
-        <f>IF(V48="","",IF(F48=0,0,1+2*V48))</f>
+        <f t="shared" ref="AV48:BD48" si="52">IF(V48="","",IF(F48=0,0,1+2*V48))</f>
         <v/>
       </c>
       <c r="AW48" s="78" t="str">
-        <f>IF(W48="","",IF(G48=0,0,1+2*W48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="AX48" s="78" t="str">
-        <f>IF(X48="","",IF(H48=0,0,1+2*X48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="AY48" s="78" t="str">
-        <f>IF(Y48="","",IF(I48=0,0,1+2*Y48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="AZ48" s="78" t="str">
-        <f>IF(Z48="","",IF(J48=0,0,1+2*Z48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="BA48" s="78" t="str">
-        <f>IF(AA48="","",IF(K48=0,0,1+2*AA48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="BB48" s="78" t="str">
-        <f>IF(AB48="","",IF(L48=0,0,1+2*AB48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="BC48" s="78" t="str">
-        <f>IF(AC48="","",IF(M48=0,0,1+2*AC48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
       <c r="BD48" s="79" t="str">
-        <f>IF(AD48="","",IF(N48=0,0,1+2*AD48))</f>
+        <f t="shared" si="52"/>
         <v/>
       </c>
     </row>
@@ -10435,7 +10454,7 @@
       <c r="M49" s="34"/>
       <c r="N49" s="34"/>
       <c r="O49" s="35">
-        <f>SUM(C49:N49)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P49" s="36">
@@ -10443,7 +10462,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="36">
-        <f>COUNT(C49:N49)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R49" s="45"/>
@@ -10542,50 +10561,50 @@
         <v>0</v>
       </c>
       <c r="AS49" s="77" t="str">
-        <f>IF(S49="","",IF(C49=0,0,1+2*S49))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT49" s="78" t="str">
-        <f>IF(T49="","",IF(D49=0,0,1+2*T49))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU49" s="78" t="str">
-        <f>IF(U49="","",IF(E49=0,0,1+2*U49))</f>
+        <f t="shared" ref="AU49:AU57" si="53">IF(U49="","",IF(E49=0,0,1+2*U49))</f>
         <v/>
       </c>
       <c r="AV49" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AW49" s="78" t="str">
-        <f>IF(W49="","",IF(G49=0,0,1+2*W49))</f>
+        <f t="shared" ref="AW49:BD49" si="54">IF(W49="","",IF(G49=0,0,1+2*W49))</f>
         <v/>
       </c>
       <c r="AX49" s="78" t="str">
-        <f>IF(X49="","",IF(H49=0,0,1+2*X49))</f>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="AY49" s="78" t="str">
-        <f>IF(Y49="","",IF(I49=0,0,1+2*Y49))</f>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="AZ49" s="78" t="str">
-        <f>IF(Z49="","",IF(J49=0,0,1+2*Z49))</f>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="BA49" s="78" t="str">
-        <f>IF(AA49="","",IF(K49=0,0,1+2*AA49))</f>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="BB49" s="78" t="str">
-        <f>IF(AB49="","",IF(L49=0,0,1+2*AB49))</f>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="BC49" s="78" t="str">
-        <f>IF(AC49="","",IF(M49=0,0,1+2*AC49))</f>
+        <f t="shared" si="54"/>
         <v/>
       </c>
       <c r="BD49" s="79" t="str">
-        <f>IF(AD49="","",IF(N49=0,0,1+2*AD49))</f>
+        <f t="shared" si="54"/>
         <v/>
       </c>
     </row>
@@ -10609,7 +10628,7 @@
       <c r="M50" s="34"/>
       <c r="N50" s="34"/>
       <c r="O50" s="35">
-        <f>SUM(C50:N50)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P50" s="36">
@@ -10617,7 +10636,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="36">
-        <f>COUNT(C50:N50)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R50" s="45"/>
@@ -10716,50 +10735,50 @@
         <v>0</v>
       </c>
       <c r="AS50" s="77" t="str">
-        <f>IF(S50="","",IF(C50=0,0,1+2*S50))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT50" s="78" t="str">
-        <f>IF(T50="","",IF(D50=0,0,1+2*T50))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU50" s="78" t="str">
-        <f>IF(U50="","",IF(E50=0,0,1+2*U50))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV50" s="78" t="str">
-        <f>IF(V50="","",IF(F50=0,0,1+2*V50))</f>
+        <f t="shared" ref="AV50:AV57" si="55">IF(V50="","",IF(F50=0,0,1+2*V50))</f>
         <v/>
       </c>
       <c r="AW50" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AX50" s="78" t="str">
-        <f>IF(X50="","",IF(H50=0,0,1+2*X50))</f>
+        <f t="shared" ref="AX50:BD50" si="56">IF(X50="","",IF(H50=0,0,1+2*X50))</f>
         <v/>
       </c>
       <c r="AY50" s="78" t="str">
-        <f>IF(Y50="","",IF(I50=0,0,1+2*Y50))</f>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="AZ50" s="78" t="str">
-        <f>IF(Z50="","",IF(J50=0,0,1+2*Z50))</f>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="BA50" s="78" t="str">
-        <f>IF(AA50="","",IF(K50=0,0,1+2*AA50))</f>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="BB50" s="78" t="str">
-        <f>IF(AB50="","",IF(L50=0,0,1+2*AB50))</f>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="BC50" s="78" t="str">
-        <f>IF(AC50="","",IF(M50=0,0,1+2*AC50))</f>
+        <f t="shared" si="56"/>
         <v/>
       </c>
       <c r="BD50" s="79" t="str">
-        <f>IF(AD50="","",IF(N50=0,0,1+2*AD50))</f>
+        <f t="shared" si="56"/>
         <v/>
       </c>
     </row>
@@ -10783,7 +10802,7 @@
       <c r="M51" s="34"/>
       <c r="N51" s="34"/>
       <c r="O51" s="35">
-        <f>SUM(C51:N51)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P51" s="36">
@@ -10791,7 +10810,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="36">
-        <f>COUNT(C51:N51)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R51" s="45"/>
@@ -10890,50 +10909,50 @@
         <v>0</v>
       </c>
       <c r="AS51" s="77" t="str">
-        <f>IF(S51="","",IF(C51=0,0,1+2*S51))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT51" s="78" t="str">
-        <f>IF(T51="","",IF(D51=0,0,1+2*T51))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU51" s="78" t="str">
-        <f>IF(U51="","",IF(E51=0,0,1+2*U51))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV51" s="78" t="str">
-        <f>IF(V51="","",IF(F51=0,0,1+2*V51))</f>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="AW51" s="78" t="str">
-        <f>IF(W51="","",IF(G51=0,0,1+2*W51))</f>
+        <f t="shared" ref="AW51:AW57" si="57">IF(W51="","",IF(G51=0,0,1+2*W51))</f>
         <v/>
       </c>
       <c r="AX51" s="78" t="s">
         <v>37</v>
       </c>
       <c r="AY51" s="78" t="str">
-        <f>IF(Y51="","",IF(I51=0,0,1+2*Y51))</f>
+        <f t="shared" ref="AY51:BD51" si="58">IF(Y51="","",IF(I51=0,0,1+2*Y51))</f>
         <v/>
       </c>
       <c r="AZ51" s="78" t="str">
-        <f>IF(Z51="","",IF(J51=0,0,1+2*Z51))</f>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="BA51" s="78" t="str">
-        <f>IF(AA51="","",IF(K51=0,0,1+2*AA51))</f>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="BB51" s="78" t="str">
-        <f>IF(AB51="","",IF(L51=0,0,1+2*AB51))</f>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="BC51" s="78" t="str">
-        <f>IF(AC51="","",IF(M51=0,0,1+2*AC51))</f>
+        <f t="shared" si="58"/>
         <v/>
       </c>
       <c r="BD51" s="79" t="str">
-        <f>IF(AD51="","",IF(N51=0,0,1+2*AD51))</f>
+        <f t="shared" si="58"/>
         <v/>
       </c>
     </row>
@@ -10957,7 +10976,7 @@
       <c r="M52" s="34"/>
       <c r="N52" s="34"/>
       <c r="O52" s="35">
-        <f>SUM(C52:N52)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P52" s="36">
@@ -10965,7 +10984,7 @@
         <v>0</v>
       </c>
       <c r="Q52" s="36">
-        <f>COUNT(C52:N52)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R52" s="45"/>
@@ -11064,27 +11083,27 @@
         <v>0</v>
       </c>
       <c r="AS52" s="77" t="str">
-        <f>IF(S52="","",IF(C52=0,0,1+2*S52))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT52" s="78" t="str">
-        <f>IF(T52="","",IF(D52=0,0,1+2*T52))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU52" s="78" t="str">
-        <f>IF(U52="","",IF(E52=0,0,1+2*U52))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV52" s="78" t="str">
-        <f>IF(V52="","",IF(F52=0,0,1+2*V52))</f>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="AW52" s="78" t="str">
-        <f>IF(W52="","",IF(G52=0,0,1+2*W52))</f>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="AX52" s="78" t="str">
-        <f>IF(X52="","",IF(H52=0,0,1+2*X52))</f>
+        <f t="shared" ref="AX52:AX57" si="59">IF(X52="","",IF(H52=0,0,1+2*X52))</f>
         <v/>
       </c>
       <c r="AY52" s="78" t="s">
@@ -11131,7 +11150,7 @@
       <c r="M53" s="34"/>
       <c r="N53" s="34"/>
       <c r="O53" s="35">
-        <f>SUM(C53:N53)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P53" s="36">
@@ -11139,7 +11158,7 @@
         <v>0</v>
       </c>
       <c r="Q53" s="36">
-        <f>COUNT(C53:N53)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R53" s="45"/>
@@ -11238,27 +11257,27 @@
         <v>0</v>
       </c>
       <c r="AS53" s="77" t="str">
-        <f>IF(S53="","",IF(C53=0,0,1+2*S53))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT53" s="78" t="str">
-        <f>IF(T53="","",IF(D53=0,0,1+2*T53))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU53" s="78" t="str">
-        <f>IF(U53="","",IF(E53=0,0,1+2*U53))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV53" s="78" t="str">
-        <f>IF(V53="","",IF(F53=0,0,1+2*V53))</f>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="AW53" s="78" t="str">
-        <f>IF(W53="","",IF(G53=0,0,1+2*W53))</f>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="AX53" s="78" t="str">
-        <f>IF(X53="","",IF(H53=0,0,1+2*X53))</f>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AY53" s="78" t="str">
@@ -11305,7 +11324,7 @@
       <c r="M54" s="34"/>
       <c r="N54" s="34"/>
       <c r="O54" s="35">
-        <f>SUM(C54:N54)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P54" s="36">
@@ -11313,7 +11332,7 @@
         <v>0</v>
       </c>
       <c r="Q54" s="36">
-        <f>COUNT(C54:N54)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R54" s="45"/>
@@ -11412,27 +11431,27 @@
         <v>0</v>
       </c>
       <c r="AS54" s="77" t="str">
-        <f>IF(S54="","",IF(C54=0,0,1+2*S54))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT54" s="78" t="str">
-        <f>IF(T54="","",IF(D54=0,0,1+2*T54))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU54" s="78" t="str">
-        <f>IF(U54="","",IF(E54=0,0,1+2*U54))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV54" s="78" t="str">
-        <f>IF(V54="","",IF(F54=0,0,1+2*V54))</f>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="AW54" s="78" t="str">
-        <f>IF(W54="","",IF(G54=0,0,1+2*W54))</f>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="AX54" s="78" t="str">
-        <f>IF(X54="","",IF(H54=0,0,1+2*X54))</f>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AY54" s="78" t="str">
@@ -11479,7 +11498,7 @@
       <c r="M55" s="34"/>
       <c r="N55" s="34"/>
       <c r="O55" s="35">
-        <f>SUM(C55:N55)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P55" s="36">
@@ -11487,7 +11506,7 @@
         <v>0</v>
       </c>
       <c r="Q55" s="36">
-        <f>COUNT(C55:N55)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R55" s="45"/>
@@ -11586,27 +11605,27 @@
         <v>0</v>
       </c>
       <c r="AS55" s="77" t="str">
-        <f>IF(S55="","",IF(C55=0,0,1+2*S55))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT55" s="78" t="str">
-        <f>IF(T55="","",IF(D55=0,0,1+2*T55))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU55" s="78" t="str">
-        <f>IF(U55="","",IF(E55=0,0,1+2*U55))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV55" s="78" t="str">
-        <f>IF(V55="","",IF(F55=0,0,1+2*V55))</f>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="AW55" s="78" t="str">
-        <f>IF(W55="","",IF(G55=0,0,1+2*W55))</f>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="AX55" s="78" t="str">
-        <f>IF(X55="","",IF(H55=0,0,1+2*X55))</f>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AY55" s="78" t="str">
@@ -11653,7 +11672,7 @@
       </c>
       <c r="N56" s="34"/>
       <c r="O56" s="35">
-        <f>SUM(C56:N56)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P56" s="36">
@@ -11661,7 +11680,7 @@
         <v>0</v>
       </c>
       <c r="Q56" s="36">
-        <f>COUNT(C56:N56)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R56" s="45"/>
@@ -11760,27 +11779,27 @@
         <v>0</v>
       </c>
       <c r="AS56" s="77" t="str">
-        <f>IF(S56="","",IF(C56=0,0,1+2*S56))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT56" s="78" t="str">
-        <f>IF(T56="","",IF(D56=0,0,1+2*T56))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU56" s="78" t="str">
-        <f>IF(U56="","",IF(E56=0,0,1+2*U56))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV56" s="78" t="str">
-        <f>IF(V56="","",IF(F56=0,0,1+2*V56))</f>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="AW56" s="78" t="str">
-        <f>IF(W56="","",IF(G56=0,0,1+2*W56))</f>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="AX56" s="78" t="str">
-        <f>IF(X56="","",IF(H56=0,0,1+2*X56))</f>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AY56" s="78" t="str">
@@ -11827,7 +11846,7 @@
         <v>37</v>
       </c>
       <c r="O57" s="41">
-        <f>SUM(C57:N57)</f>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="P57" s="42">
@@ -11835,7 +11854,7 @@
         <v>0</v>
       </c>
       <c r="Q57" s="42">
-        <f>COUNT(C57:N57)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R57" s="45"/>
@@ -11934,27 +11953,27 @@
         <v>37</v>
       </c>
       <c r="AS57" s="80" t="str">
-        <f>IF(S57="","",IF(C57=0,0,1+2*S57))</f>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="AT57" s="81" t="str">
-        <f>IF(T57="","",IF(D57=0,0,1+2*T57))</f>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="AU57" s="81" t="str">
-        <f>IF(U57="","",IF(E57=0,0,1+2*U57))</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="AV57" s="81" t="str">
-        <f>IF(V57="","",IF(F57=0,0,1+2*V57))</f>
+        <f t="shared" si="55"/>
         <v/>
       </c>
       <c r="AW57" s="81" t="str">
-        <f>IF(W57="","",IF(G57=0,0,1+2*W57))</f>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="AX57" s="81" t="str">
-        <f>IF(X57="","",IF(H57=0,0,1+2*X57))</f>
+        <f t="shared" si="59"/>
         <v/>
       </c>
       <c r="AY57" s="81" t="str">

</xml_diff>